<commit_message>
change the sheet name of demo_lists.xlsx
</commit_message>
<xml_diff>
--- a/source/chapters/demo_lists.xlsx
+++ b/source/chapters/demo_lists.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -732,7 +732,7 @@
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>